<commit_message>
coding cleaning script to fix up the raw data from the experts.  UGGHHHH
Former-commit-id: 559a6a38fe91d8d131903d3f6cc8ccf06c9191c4
</commit_message>
<xml_diff>
--- a/_raw_data/xlsx/cat_val_key_tidyish.xlsx
+++ b/_raw_data/xlsx/cat_val_key_tidyish.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="109">
   <si>
     <t>Category</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>sessile, nearly sessile/sedentary, passive, vertical migrator, mobile resident, horizontal migrator, nomadic</t>
-  </si>
-  <si>
-    <t>planktonic larval duration (PLD)</t>
   </si>
   <si>
     <r>
@@ -72,9 +69,6 @@
   </si>
   <si>
     <t>lifetime # reproductive opportunities</t>
-  </si>
-  <si>
-    <t>1, 2-10, 11-25, 26-50, 51-100, 100+</t>
   </si>
   <si>
     <t>age to 1st reproduction/generation time</t>
@@ -377,9 +371,6 @@
     <t>extreme pressure wave sensitive structures</t>
   </si>
   <si>
-    <t>high; medium; low sensitivity</t>
-  </si>
-  <si>
     <t>respiration structures</t>
   </si>
   <si>
@@ -466,12 +457,6 @@
     <t>sexual dioecious; sexual hermaphrodite; asexual; colonial</t>
   </si>
   <si>
-    <t xml:space="preserve"> 1-2; 2-5; 5-10; 10-20; 20-50; 50-100; 100-1000; 1000-10,000; &gt;10,000</t>
-  </si>
-  <si>
-    <t>1; 2-10; 11-25; 26-50; 51-100; 100+</t>
-  </si>
-  <si>
     <t>feeding; non-feeding; no larva; NA</t>
   </si>
   <si>
@@ -539,6 +524,24 @@
   </si>
   <si>
     <t>live birth/ egg care; spawner; egg-layer; egg-layer (unattended)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &gt;1000 mm; 50 mm-999 mm; 0.5mm-49 mm; &lt;0.4 mm</t>
+  </si>
+  <si>
+    <t>planktonic larval duration (PLD) exposure</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;1; 1-2; 2-5; 5-10; 10-20; 20-50; 50-100; 100-1000; 1000-10,000; &gt;10,000</t>
+  </si>
+  <si>
+    <t>high; medium; low; none</t>
+  </si>
+  <si>
+    <t>1, 2-10, 11-25, 26-50, 51-100, &gt;100</t>
+  </si>
+  <si>
+    <t>1; 2-10; 11-25; 26-50; 51-100; &gt;100</t>
   </si>
 </sst>
 </file>
@@ -1021,7 +1024,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1032,7 +1035,7 @@
   <dimension ref="A1:D74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1048,18 +1051,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -1068,537 +1071,537 @@
         <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="D3" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="D5" s="4" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>107</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="5"/>
       <c r="B11" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="D28" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2"/>
       <c r="B29" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="16">
       <c r="A34" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>60</v>
-      </c>
       <c r="D34" s="7" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2"/>
       <c r="B35" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>65</v>
-      </c>
       <c r="D37" s="5" t="s">
-        <v>65</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2"/>
       <c r="B38" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2"/>
       <c r="B40" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2"/>
       <c r="B42" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2"/>
       <c r="B43" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2"/>
       <c r="B44" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2"/>
       <c r="B45" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="48" spans="1:4">

</xml_diff>